<commit_message>
Change implementation of some parameters
</commit_message>
<xml_diff>
--- a/src/configurations_param.xlsx
+++ b/src/configurations_param.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,13 +483,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5554648000000002</v>
+        <v>0.09945599999999999</v>
       </c>
     </row>
     <row r="3">
@@ -500,7 +500,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>crossover_one_point</t>
+          <t>crossover_two_point</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -509,24 +509,24 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.01212380000000213</v>
+        <v>0.0003959999999998409</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>best_of_all_selection</t>
+          <t>tournament_selection</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>crossover_one_point</t>
+          <t>crossover_homogenous</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -535,299 +535,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="E4" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002063999999997179</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>best_of_all_selection</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>crossover_one_point</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>400</v>
-      </c>
-      <c r="E5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-0.0009273999999948046</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>best_of_all_selection</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>400</v>
-      </c>
-      <c r="E6" t="n">
-        <v>20</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.02238349999999656</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>best_of_all_selection</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>400</v>
-      </c>
-      <c r="E7" t="n">
-        <v>20</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-0.01020479999999679</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>tournament_selection</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>400</v>
-      </c>
-      <c r="E8" t="n">
-        <v>20</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.09559949999999873</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>tournament_selection</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>400</v>
-      </c>
-      <c r="E9" t="n">
-        <v>20</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-0.03269499999999681</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>best_of_all_selection</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>400</v>
-      </c>
-      <c r="E10" t="n">
-        <v>20</v>
-      </c>
-      <c r="F10" t="n">
-        <v>-0.05899700000000507</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>best_of_all_selection</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>400</v>
-      </c>
-      <c r="E11" t="n">
-        <v>20</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.008810599999989677</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>tournament_selection</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>400</v>
-      </c>
-      <c r="E12" t="n">
-        <v>20</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.01331740000003379</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>roulette_wheel_selection</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>200</v>
-      </c>
-      <c r="E13" t="n">
-        <v>20</v>
-      </c>
-      <c r="F13" t="n">
-        <v>2.968632099999979</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>roulette_wheel_selection</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>200</v>
-      </c>
-      <c r="E14" t="n">
-        <v>20</v>
-      </c>
-      <c r="F14" t="n">
-        <v>2.925955999999985</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>best_of_all_selection</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>crossover_two_point</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>two_points_mutation</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>200</v>
-      </c>
-      <c r="E15" t="n">
-        <v>20</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-6.190125199999983</v>
+        <v>0.01830899999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added real values algorithm usage
</commit_message>
<xml_diff>
--- a/src/configurations_param.xlsx
+++ b/src/configurations_param.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,12 +474,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>crossover_one_point</t>
+          <t>real_values_crossover_heurestic</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>edge_mutation</t>
+          <t>real_values_uniform_mutation</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -489,7 +489,7 @@
         <v>50</v>
       </c>
       <c r="F2" t="n">
-        <v>0.09945599999999999</v>
+        <v>0.05789840000000268</v>
       </c>
     </row>
     <row r="3">
@@ -500,12 +500,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>crossover_two_point</t>
+          <t>real_values_crossover_heurestic</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>edge_mutation</t>
+          <t>real_values_uniform_mutation</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,23 +515,23 @@
         <v>50</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0003959999999998409</v>
+        <v>-0.003664900000003968</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>tournament_selection</t>
+          <t>best_of_all_selection</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>crossover_homogenous</t>
+          <t>real_values_crossover_heurestic</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>two_points_mutation</t>
+          <t>real_values_uniform_mutation</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -541,7 +541,475 @@
         <v>50</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01830899999999991</v>
+        <v>-0.003326200000000057</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" t="n">
+        <v>50</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.005946800000003805</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.006491099999998085</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>50</v>
+      </c>
+      <c r="E7" t="n">
+        <v>50</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.00386599999999504</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>50</v>
+      </c>
+      <c r="E8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.001894900000003474</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>50</v>
+      </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.0007946999999859372</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>50</v>
+      </c>
+      <c r="E10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.004845499999987624</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>50</v>
+      </c>
+      <c r="E11" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.003720899999990479</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>50</v>
+      </c>
+      <c r="E12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.001389699999990057</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>50</v>
+      </c>
+      <c r="E13" t="n">
+        <v>50</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.002035599999999249</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>50</v>
+      </c>
+      <c r="E14" t="n">
+        <v>50</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.002667100000010691</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>50</v>
+      </c>
+      <c r="E15" t="n">
+        <v>50</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.01978369999999074</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>50</v>
+      </c>
+      <c r="E16" t="n">
+        <v>50</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.02319819999999595</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>50</v>
+      </c>
+      <c r="E17" t="n">
+        <v>50</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.001183900000000904</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>500</v>
+      </c>
+      <c r="E18" t="n">
+        <v>50</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.480582499999997</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>500</v>
+      </c>
+      <c r="E19" t="n">
+        <v>50</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.008589999999998099</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>500</v>
+      </c>
+      <c r="E20" t="n">
+        <v>50</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.04207550000000992</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>50</v>
+      </c>
+      <c r="E21" t="n">
+        <v>50</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-0.527860600000011</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>best_of_all_selection</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>real_values_crossover_heurestic</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>real_values_uniform_mutation</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>50</v>
+      </c>
+      <c r="E22" t="n">
+        <v>50</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0002268000000071879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>